<commit_message>
updates to part 3 analysis
</commit_message>
<xml_diff>
--- a/part_3_cohere/analysis/dense_analysis_results_data.xlsx
+++ b/part_3_cohere/analysis/dense_analysis_results_data.xlsx
@@ -8,23 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/poppyriddle/Documents/Github/Research_proposal/part_3_cohere/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE08AC7A-B3AF-A64D-9225-0B6ADB490A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91C5045-21BF-0B4B-B91A-F43E9BDE77EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="760" windowWidth="30060" windowHeight="18880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="760" windowWidth="30060" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="avg scores" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="avg doc score" sheetId="3" r:id="rId3"/>
+    <sheet name="precision" sheetId="4" r:id="rId2"/>
+    <sheet name="raw data" sheetId="1" r:id="rId3"/>
+    <sheet name="avg doc score" sheetId="3" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId6"/>
-    <pivotCache cacheId="31" r:id="rId7"/>
+    <pivotCache cacheId="9" r:id="rId7"/>
+    <pivotCache cacheId="31" r:id="rId8"/>
+    <pivotCache cacheId="43" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="155">
   <si>
     <t>Query</t>
   </si>
@@ -930,10 +932,22 @@
     <t>Average of Documents score:data_multi_lang</t>
   </si>
   <si>
+    <t>StdDev of Documents score</t>
+  </si>
+  <si>
     <t>Max of Documents score</t>
   </si>
   <si>
     <t>Min of Documents score</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>Min of Precision</t>
+  </si>
+  <si>
+    <t>Max of Precision</t>
   </si>
 </sst>
 </file>
@@ -1037,25 +1051,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.00000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="0.0000"/>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <numFmt numFmtId="171" formatCode="0.0000"/>
     </dxf>
@@ -4198,8 +4194,8 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -4234,8 +4230,8 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
       <xdr:row>96</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -4273,13 +4269,15 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="avg scores"/>
-      <sheetName val="Sheet1"/>
+      <sheetName val="precision"/>
+      <sheetName val="raw data"/>
       <sheetName val="avg doc score"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3">
         <row r="1">
           <cell r="E1" t="str">
             <v>Row Labels</v>
@@ -4534,250 +4532,252 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="avg scores"/>
-      <sheetName val="Sheet1"/>
+      <sheetName val="precision"/>
+      <sheetName val="raw data"/>
       <sheetName val="avg doc score"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="266">
-          <cell r="E266" t="str">
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3">
+        <row r="1">
+          <cell r="E1" t="str">
             <v>Row Labels- data_multi_lang</v>
           </cell>
-          <cell r="F266" t="str">
+          <cell r="F1" t="str">
             <v>Average of Documents score:data_multi_lang</v>
           </cell>
         </row>
-        <row r="267">
-          <cell r="E267" t="str">
+        <row r="2">
+          <cell r="E2" t="str">
             <v xml:space="preserve"> 10.1002/leap.1411</v>
           </cell>
-          <cell r="F267">
+          <cell r="F2">
             <v>0.14053692000000001</v>
           </cell>
         </row>
-        <row r="268">
-          <cell r="E268" t="str">
+        <row r="3">
+          <cell r="E3" t="str">
             <v xml:space="preserve"> 10.1007/978-3-031-88708-6_3</v>
           </cell>
-          <cell r="F268">
+          <cell r="F3">
             <v>0.73398845000000013</v>
           </cell>
         </row>
-        <row r="269">
-          <cell r="E269" t="str">
+        <row r="4">
+          <cell r="E4" t="str">
             <v xml:space="preserve"> 10.1007/s11192-015-1765-5</v>
           </cell>
-          <cell r="F269">
+          <cell r="F4">
             <v>0.40059755499999994</v>
           </cell>
         </row>
-        <row r="270">
-          <cell r="E270" t="str">
+        <row r="5">
+          <cell r="E5" t="str">
             <v xml:space="preserve"> 10.1007/s11192-022-04367-w</v>
           </cell>
-          <cell r="F270">
+          <cell r="F5">
             <v>0.2380918345000001</v>
           </cell>
         </row>
-        <row r="271">
-          <cell r="E271" t="str">
+        <row r="6">
+          <cell r="E6" t="str">
             <v xml:space="preserve"> 10.1007/s11192-023-04923-y</v>
           </cell>
-          <cell r="F271">
+          <cell r="F6">
             <v>0.69294593199999999</v>
           </cell>
         </row>
-        <row r="272">
-          <cell r="E272" t="str">
+        <row r="7">
+          <cell r="E7" t="str">
             <v xml:space="preserve"> 10.1162/qss_a_00022</v>
           </cell>
-          <cell r="F272">
+          <cell r="F7">
             <v>0.8639597349999999</v>
           </cell>
         </row>
-        <row r="273">
-          <cell r="E273" t="str">
+        <row r="8">
+          <cell r="E8" t="str">
             <v xml:space="preserve"> 10.1162/qss_a_00112</v>
           </cell>
-          <cell r="F273">
+          <cell r="F8">
             <v>0.24088813749999999</v>
           </cell>
         </row>
-        <row r="274">
-          <cell r="E274" t="str">
+        <row r="9">
+          <cell r="E9" t="str">
             <v xml:space="preserve"> 10.1162/qss_a_00210</v>
           </cell>
-          <cell r="F274">
+          <cell r="F9">
             <v>0.60251958000000017</v>
           </cell>
         </row>
-        <row r="275">
-          <cell r="E275" t="str">
+        <row r="10">
+          <cell r="E10" t="str">
             <v xml:space="preserve"> 10.1162/qss_a_00212</v>
           </cell>
-          <cell r="F275">
+          <cell r="F10">
             <v>0.39641916999999999</v>
           </cell>
         </row>
-        <row r="276">
-          <cell r="E276" t="str">
+        <row r="11">
+          <cell r="E11" t="str">
             <v xml:space="preserve"> 10.1162/qss_a_00286</v>
           </cell>
-          <cell r="F276">
+          <cell r="F11">
             <v>0.44670673666666671</v>
           </cell>
         </row>
-        <row r="277">
-          <cell r="E277" t="str">
+        <row r="12">
+          <cell r="E12" t="str">
             <v xml:space="preserve"> 10.1371/journal.pbio.1002542</v>
           </cell>
-          <cell r="F277">
+          <cell r="F12">
             <v>0.52339156499999984</v>
           </cell>
         </row>
-        <row r="278">
-          <cell r="E278" t="str">
+        <row r="13">
+          <cell r="E13" t="str">
             <v xml:space="preserve"> 10.1609/aaai.v38i16.29728</v>
           </cell>
-          <cell r="F278">
+          <cell r="F13">
             <v>0.89763280000000001</v>
           </cell>
         </row>
-        <row r="279">
-          <cell r="E279" t="str">
+        <row r="14">
+          <cell r="E14" t="str">
             <v xml:space="preserve"> 10.31222/osf.io/smxe5</v>
           </cell>
-          <cell r="F279">
+          <cell r="F14">
             <v>0.40011453249999995</v>
           </cell>
         </row>
-        <row r="280">
-          <cell r="E280" t="str">
+        <row r="15">
+          <cell r="E15" t="str">
             <v xml:space="preserve"> 10.31274/b8136f97.ccc3dae4</v>
           </cell>
-          <cell r="F280">
+          <cell r="F15">
             <v>0.37355851499999998</v>
           </cell>
         </row>
-        <row r="281">
-          <cell r="E281" t="str">
+        <row r="16">
+          <cell r="E16" t="str">
             <v xml:space="preserve"> 10.3145/epi.2023.mar.09</v>
           </cell>
-          <cell r="F281">
+          <cell r="F16">
             <v>0.50971825733333342</v>
           </cell>
         </row>
-        <row r="282">
-          <cell r="E282" t="str">
+        <row r="17">
+          <cell r="E17" t="str">
             <v xml:space="preserve"> 10.48550/arXiv.2303.17661</v>
           </cell>
-          <cell r="F282">
+          <cell r="F17">
             <v>0.33921495000000002</v>
           </cell>
         </row>
-        <row r="283">
-          <cell r="E283" t="str">
+        <row r="18">
+          <cell r="E18" t="str">
             <v xml:space="preserve"> 10.48550/arXiv.2312.10997</v>
           </cell>
-          <cell r="F283">
+          <cell r="F18">
             <v>0.63463328333333313</v>
           </cell>
         </row>
-        <row r="284">
-          <cell r="E284" t="str">
+        <row r="19">
+          <cell r="E19" t="str">
             <v xml:space="preserve"> 10.48550/arXiv.2401.16359</v>
           </cell>
-          <cell r="F284">
+          <cell r="F19">
             <v>0.50976659499999999</v>
           </cell>
         </row>
-        <row r="285">
-          <cell r="E285" t="str">
+        <row r="20">
+          <cell r="E20" t="str">
             <v xml:space="preserve"> 10.48550/arXiv.2404.01985</v>
           </cell>
-          <cell r="F285">
+          <cell r="F20">
             <v>0.15831774000000001</v>
           </cell>
         </row>
-        <row r="286">
-          <cell r="E286" t="str">
+        <row r="21">
+          <cell r="E21" t="str">
             <v xml:space="preserve"> 10.48550/arXiv.2404.13948</v>
           </cell>
-          <cell r="F286">
+          <cell r="F21">
             <v>0.59891786999999996</v>
           </cell>
         </row>
-        <row r="287">
-          <cell r="E287" t="str">
+        <row r="22">
+          <cell r="E22" t="str">
             <v xml:space="preserve"> 10.48550/arXiv.2404.17663</v>
           </cell>
-          <cell r="F287">
+          <cell r="F22">
             <v>0.62186232499999983</v>
           </cell>
         </row>
-        <row r="288">
-          <cell r="E288" t="str">
+        <row r="23">
+          <cell r="E23" t="str">
             <v xml:space="preserve"> 10.48550/arXiv.2406.13213</v>
           </cell>
-          <cell r="F288">
+          <cell r="F23">
             <v>0.66593574999999994</v>
           </cell>
         </row>
-        <row r="289">
-          <cell r="E289" t="str">
+        <row r="24">
+          <cell r="E24" t="str">
             <v xml:space="preserve"> 10.48550/arXiv.2406.15154</v>
           </cell>
-          <cell r="F289">
+          <cell r="F24">
             <v>0.63443416599999991</v>
           </cell>
         </row>
-        <row r="290">
-          <cell r="E290" t="str">
+        <row r="25">
+          <cell r="E25" t="str">
             <v xml:space="preserve"> 10.48550/arXiv.2409.10633</v>
           </cell>
-          <cell r="F290">
+          <cell r="F25">
             <v>0.71322715500000045</v>
           </cell>
         </row>
-        <row r="291">
-          <cell r="E291" t="str">
+        <row r="26">
+          <cell r="E26" t="str">
             <v xml:space="preserve"> 10.48550/arXiv.2410.04231</v>
           </cell>
-          <cell r="F291">
+          <cell r="F26">
             <v>0.88611550000000006</v>
           </cell>
         </row>
-        <row r="292">
-          <cell r="E292" t="str">
+        <row r="27">
+          <cell r="E27" t="str">
             <v xml:space="preserve"> 10.48550/arXiv.2505.18247</v>
           </cell>
-          <cell r="F292">
+          <cell r="F27">
             <v>0.51829862500000012</v>
           </cell>
         </row>
-        <row r="293">
-          <cell r="E293" t="str">
+        <row r="28">
+          <cell r="E28" t="str">
             <v xml:space="preserve"> 10.5281/ZENODO.13960973</v>
           </cell>
-          <cell r="F293">
+          <cell r="F28">
             <v>0.74895920000000005</v>
           </cell>
         </row>
-        <row r="294">
-          <cell r="E294" t="str">
+        <row r="29">
+          <cell r="E29" t="str">
             <v xml:space="preserve"> 10.6109/jkiice.2023.27.12.1489</v>
           </cell>
-          <cell r="F294">
+          <cell r="F29">
             <v>0.75809943999999996</v>
           </cell>
         </row>
-        <row r="295">
-          <cell r="E295" t="str">
+        <row r="30">
+          <cell r="E30" t="str">
             <v>Grand Total</v>
           </cell>
-          <cell r="F295">
+          <cell r="F30">
             <v>0.52488956619354721</v>
           </cell>
         </row>
@@ -4790,7 +4790,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Poppy Riddle" refreshedDate="45914.568360300924" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="70" xr:uid="{8054517A-DDCD-A746-9F4D-0716BA9D1C69}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="B1:J71" sheet="Sheet1"/>
+    <worksheetSource ref="B1:J71" sheet="raw data"/>
   </cacheSource>
   <cacheFields count="9">
     <cacheField name="Query" numFmtId="0">
@@ -4985,6 +4985,58 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Poppy Riddle" refreshedDate="45914.618390509262" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="71" xr:uid="{2348D42D-E7B2-A245-B7D8-CDBFDDA5D8B5}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B1:H1048576" sheet="raw data"/>
+  </cacheSource>
+  <cacheFields count="7">
+    <cacheField name="Query" numFmtId="0">
+      <sharedItems containsBlank="1" count="15">
+        <s v="which studies examined the abstract in metadata?"/>
+        <s v="which studies examined citations?"/>
+        <s v="Tell me about OpenAlex."/>
+        <s v="Tell me about Crossref."/>
+        <s v="Which papers evaluate the linguistic coverage or language-related metadata in scholarly databases?"/>
+        <s v="Which papers address funding metadata, its availability, or its analysis in scholarly databases?"/>
+        <s v="Which papers discuss the use of Retrieval-Augmented Generation (RAG) in large language models or related applications?"/>
+        <s v="What is Crossref’s role in the scholarly research ecosystem?"/>
+        <s v="What are the key features and limitations of OpenAlex as a bibliometric database?"/>
+        <s v="What are the strengths and weaknesses of Web of Science (WoS) as a bibliometric database?"/>
+        <s v="How is RAG used to improve question answering or information retrieval systems?"/>
+        <s v="What are the main challenges in normalizing citation metrics across scientific fields?"/>
+        <s v="What methods are used to detect and correct errors in bibliographic datasets?"/>
+        <s v="tell me about how RAG works."/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Precision" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="1"/>
+    </cacheField>
+    <cacheField name="Recall" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="1"/>
+    </cacheField>
+    <cacheField name="F1-Score" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.68888888888888888" maxValue="1"/>
+    </cacheField>
+    <cacheField name="Accuracy" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.68888888888888888" maxValue="1"/>
+    </cacheField>
+    <cacheField name="Balanced accuracy" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.43055555555555558" maxValue="1"/>
+    </cacheField>
+    <cacheField name="Faithfulness score" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="5"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="70">
   <r>
@@ -6941,6 +6993,650 @@
   <r>
     <x v="68"/>
     <x v="18"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="71">
+  <r>
+    <x v="0"/>
+    <n v="0.6"/>
+    <n v="0.6"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.77499999999999991"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="0.6"/>
+    <n v="0.6"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.77499999999999991"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="0.6"/>
+    <n v="0.6"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.77499999999999991"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="0.6"/>
+    <n v="0.6"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.77499999999999991"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="0.6"/>
+    <n v="0.6"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.77499999999999991"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0.77777777777777779"/>
+    <n v="0.77777777777777779"/>
+    <n v="0.4375"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="0.4"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.7"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="0.4"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.7"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="0.4"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.7"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="0.4"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.7"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0.8"/>
+    <n v="0.8"/>
+    <n v="0.47368421052631582"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="0.8"/>
+    <n v="0.5714285714285714"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.77255639097744355"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="0.8"/>
+    <n v="0.5714285714285714"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.77255639097744355"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="0.8"/>
+    <n v="0.5714285714285714"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.77255639097744355"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="0.8"/>
+    <n v="0.5714285714285714"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.77255639097744355"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0.68888888888888888"/>
+    <n v="0.68888888888888888"/>
+    <n v="0.43055555555555558"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="0.55555555555555558"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.77777777777777779"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="0.55555555555555558"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.77777777777777779"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="0.55555555555555558"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.77777777777777779"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="0.55555555555555558"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.77777777777777779"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0.77777777777777779"/>
+    <n v="0.77777777777777779"/>
+    <n v="0.4375"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="0.6"/>
+    <n v="0.6"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.77499999999999991"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="0.6"/>
+    <n v="0.6"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.77499999999999991"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="0.6"/>
+    <n v="0.6"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.77499999999999991"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="0.6"/>
+    <n v="0.6"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.77499999999999991"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="0.4"/>
+    <n v="0.4"/>
+    <n v="0.8666666666666667"/>
+    <n v="0.8666666666666667"/>
+    <n v="0.66250000000000009"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="0.8"/>
+    <n v="0.8"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.88749999999999996"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="0.8"/>
+    <n v="0.8"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.88749999999999996"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="0.8"/>
+    <n v="0.8"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.88749999999999996"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="0.8"/>
+    <n v="0.8"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.88749999999999996"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0.77777777777777779"/>
+    <n v="0.77777777777777779"/>
+    <n v="0.4375"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="0.6"/>
+    <n v="0.6"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.77499999999999991"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="0.6"/>
+    <n v="0.6"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.77499999999999991"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="0.6"/>
+    <n v="0.6"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.77499999999999991"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="0.6"/>
+    <n v="0.6"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.77499999999999991"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0.77777777777777779"/>
+    <n v="0.77777777777777779"/>
+    <n v="0.4375"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="0.75"/>
+    <n v="0.6"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.78749999999999998"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="0.75"/>
+    <n v="0.6"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.78749999999999998"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="0.75"/>
+    <n v="0.6"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.78749999999999998"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="0.75"/>
+    <n v="0.6"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.78749999999999998"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="0.25"/>
+    <n v="0.2"/>
+    <n v="0.84444444444444444"/>
+    <n v="0.84444444444444444"/>
+    <n v="0.5625"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="0.8"/>
+    <n v="0.8"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.88749999999999996"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="0.8"/>
+    <n v="0.8"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.88749999999999996"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="0.8"/>
+    <n v="0.8"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.88749999999999996"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="0.8"/>
+    <n v="0.8"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.88749999999999996"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="0.4"/>
+    <n v="0.4"/>
+    <n v="0.8666666666666667"/>
+    <n v="0.8666666666666667"/>
+    <n v="0.66250000000000009"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="0.75"/>
+    <n v="0.6"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.78749999999999998"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="0.75"/>
+    <n v="0.6"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.78749999999999998"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="0.75"/>
+    <n v="0.6"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.78749999999999998"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="0.75"/>
+    <n v="0.6"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.93333333333333335"/>
+    <n v="0.78749999999999998"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0.8"/>
+    <n v="0.8"/>
+    <n v="0.45"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0.77777777777777779"/>
+    <n v="0.77777777777777779"/>
+    <n v="0.4375"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="1"/>
+    <n v="0.2"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.6"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="1"/>
+    <n v="0.2"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.6"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="1"/>
+    <n v="0.2"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.6"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="1"/>
+    <n v="0.2"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.6"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0.8666666666666667"/>
+    <n v="0.8666666666666667"/>
+    <n v="0.48749999999999999"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="0.66666666666666663"/>
+    <n v="0.4"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.6875"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="0.66666666666666663"/>
+    <n v="0.4"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.6875"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="0.66666666666666663"/>
+    <n v="0.4"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.6875"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="0.66666666666666663"/>
+    <n v="0.4"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.91111111111111109"/>
+    <n v="0.6875"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0.82222222222222219"/>
+    <n v="0.82222222222222219"/>
+    <n v="0.46250000000000002"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="0.8"/>
+    <n v="0.8"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.88749999999999996"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="0.8"/>
+    <n v="0.8"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.88749999999999996"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="0.8"/>
+    <n v="0.8"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.88749999999999996"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="0.8"/>
+    <n v="0.8"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.9555555555555556"/>
+    <n v="0.88749999999999996"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -7081,7 +7777,7 @@
     <dataField name="Average of Precision" fld="1" subtotal="average" baseField="0" baseItem="0" numFmtId="172"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="10">
+    <format dxfId="4">
       <pivotArea field="0" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -7090,7 +7786,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="3">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="5" selected="0">
@@ -7103,7 +7799,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="2">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -7126,8 +7822,123 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{021D7DFF-F84D-1D46-9DBB-48AA9679E9F9}" name="PivotTable11" cacheId="43" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:D19" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="16">
+        <item x="10"/>
+        <item x="3"/>
+        <item x="13"/>
+        <item x="2"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="9"/>
+        <item x="7"/>
+        <item x="12"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="14"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="16">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+  </colItems>
+  <dataFields count="3">
+    <dataField name="Min of Precision" fld="1" subtotal="min" baseField="0" baseItem="0"/>
+    <dataField name="Max of Precision" fld="1" subtotal="max" baseField="0" baseItem="0"/>
+    <dataField name="Average of Precision" fld="1" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00A3FBF8-DD41-BF4B-9469-5872331115C7}" name="PivotTable8" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="I2:K33" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <location ref="M2:O33" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
@@ -7296,9 +8107,9 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{35F14908-A910-9944-9C49-FC0167084572}" name="PivotTable5" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="D2:E33" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="D2:F33" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
@@ -7444,14 +8255,23 @@
       <x/>
     </i>
   </rowItems>
-  <colItems count="1">
-    <i/>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
   </colItems>
-  <dataFields count="1">
+  <dataFields count="2">
     <dataField name="Average of Documents score:data" fld="0" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="StdDev of Documents score" fld="0" subtotal="stdDev" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="5">
+    <format dxfId="0">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
@@ -7459,35 +8279,6 @@
       </pivotArea>
     </format>
   </formats>
-  <chartFormats count="3">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="1" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -8176,14 +8967,270 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E15C12-F878-C046-8521-C854B749CF77}">
+  <dimension ref="A3:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="93.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.69000000000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.67999999999999994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.53333333333333333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.66166666666666696</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCellId="2" sqref="I1:I1048576 B1:B1048576 A1:A1048576"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="19.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
@@ -10459,12 +11506,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C589102-22A1-C64A-88CB-289B62D6265D}">
-  <dimension ref="A1:K296"/>
+  <dimension ref="A1:O296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10473,14 +11520,15 @@
     <col min="3" max="3" width="18.5" customWidth="1"/>
     <col min="4" max="4" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.33203125" customWidth="1"/>
+    <col min="8" max="8" width="38" customWidth="1"/>
     <col min="9" max="9" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -10488,7 +11536,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0.65199819999999997</v>
       </c>
@@ -10501,23 +11549,26 @@
       <c r="E2" t="s">
         <v>146</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="J2" t="s">
-        <v>149</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0.65199819999999997</v>
       </c>
@@ -10531,24 +11582,27 @@
         <v>0.10837587200000001</v>
       </c>
       <c r="F3" s="6">
+        <v>2.531899769066102E-5</v>
+      </c>
+      <c r="G3" s="6">
         <f>_xlfn.XLOOKUP(D3,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0</v>
       </c>
-      <c r="G3" s="6">
+      <c r="H3" s="6">
         <f>_xlfn.XLOOKUP(D3,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.14053692000000001</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="J3" s="6">
+      <c r="N3" s="6">
         <v>0.10838719500000001</v>
       </c>
-      <c r="K3" s="6">
+      <c r="O3" s="6">
         <v>0.10833058</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0.65199819999999997</v>
       </c>
@@ -10561,25 +11615,28 @@
       <c r="E4" s="6">
         <v>0.17677137000000001</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G4" s="6">
         <f>_xlfn.XLOOKUP(D4,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.17389092</v>
       </c>
-      <c r="G4" s="6">
+      <c r="H4" s="6">
         <f>_xlfn.XLOOKUP(D4,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.15831774000000001</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="J4" s="6">
+      <c r="N4" s="6">
         <v>0.81909920000000003</v>
       </c>
-      <c r="K4" s="6">
+      <c r="O4" s="6">
         <v>0.63506459999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.65199819999999997</v>
       </c>
@@ -10593,24 +11650,27 @@
         <v>0.23333798466666669</v>
       </c>
       <c r="F5" s="6">
+        <v>1.76866799108381E-2</v>
+      </c>
+      <c r="G5" s="6">
         <f>_xlfn.XLOOKUP(D5,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.22407173133333333</v>
       </c>
-      <c r="G5" s="6">
+      <c r="H5" s="6">
         <f>_xlfn.XLOOKUP(D5,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.2380918345000001</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="J5" s="6">
+      <c r="N5" s="6">
         <v>0.47022631999999998</v>
       </c>
-      <c r="K5" s="6">
+      <c r="O5" s="6">
         <v>0.11645239</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.65199819999999997</v>
       </c>
@@ -10624,24 +11684,27 @@
         <v>0.24761215</v>
       </c>
       <c r="F6" s="6">
+        <v>0.11995678666827396</v>
+      </c>
+      <c r="G6" s="6">
         <f>_xlfn.XLOOKUP(D6,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.22315101999999998</v>
       </c>
-      <c r="G6" s="6">
+      <c r="H6" s="6">
         <f>_xlfn.XLOOKUP(D6,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.24088813749999999</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="J6" s="6">
+      <c r="N6" s="6">
         <v>0.25660416000000003</v>
       </c>
-      <c r="K6" s="6">
+      <c r="O6" s="6">
         <v>0.21601190000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.22735818999999999</v>
       </c>
@@ -10655,24 +11718,27 @@
         <v>0.29333935500000002</v>
       </c>
       <c r="F7" s="6">
+        <v>0.18645523259816205</v>
+      </c>
+      <c r="G7" s="6">
         <f>_xlfn.XLOOKUP(D7,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.29217876000000009</v>
       </c>
-      <c r="G7" s="6">
+      <c r="H7" s="6">
         <f>_xlfn.XLOOKUP(D7,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.40059755499999994</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="J7" s="6">
+      <c r="N7" s="6">
         <v>0.71568290000000001</v>
       </c>
-      <c r="K7" s="6">
+      <c r="O7" s="6">
         <v>0.71568290000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.22735818999999999</v>
       </c>
@@ -10686,24 +11752,27 @@
         <v>0.30744355666666667</v>
       </c>
       <c r="F8" s="6">
+        <v>0.15481180105289452</v>
+      </c>
+      <c r="G8" s="6">
         <f>_xlfn.XLOOKUP(D8,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="6">
+      <c r="H8" s="6">
         <f>_xlfn.XLOOKUP(D8,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="J8" s="6">
+      <c r="N8" s="6">
         <v>0.95696133000000005</v>
       </c>
-      <c r="K8" s="6">
+      <c r="O8" s="6">
         <v>0.74763480000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.22735818999999999</v>
       </c>
@@ -10717,24 +11786,27 @@
         <v>0.32524477800000007</v>
       </c>
       <c r="F9" s="6">
+        <v>6.6112287022570574E-3</v>
+      </c>
+      <c r="G9" s="6">
         <f>_xlfn.XLOOKUP(D9,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.30259760000000002</v>
       </c>
-      <c r="G9" s="6">
+      <c r="H9" s="6">
         <f>_xlfn.XLOOKUP(D9,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.33921495000000002</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="J9" s="6">
+      <c r="N9" s="6">
         <v>0.36141315000000002</v>
       </c>
-      <c r="K9" s="6">
+      <c r="O9" s="6">
         <v>0.13381114999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.22735818999999999</v>
       </c>
@@ -10748,24 +11820,27 @@
         <v>0.36283834733333331</v>
       </c>
       <c r="F10" s="6">
+        <v>0.13306338688582239</v>
+      </c>
+      <c r="G10" s="6">
         <f>_xlfn.XLOOKUP(D10,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.33245617249999998</v>
       </c>
-      <c r="G10" s="6">
+      <c r="H10" s="6">
         <f>_xlfn.XLOOKUP(D10,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.60251958000000017</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="J10" s="6">
+      <c r="N10" s="6">
         <v>0.53181785000000004</v>
       </c>
-      <c r="K10" s="6">
+      <c r="O10" s="6">
         <v>0.22025895000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.22735818999999999</v>
       </c>
@@ -10779,24 +11854,27 @@
         <v>0.3752652700000001</v>
       </c>
       <c r="F11" s="6">
+        <v>0.26765461119291478</v>
+      </c>
+      <c r="G11" s="6">
         <f>_xlfn.XLOOKUP(D11,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.38487724333333334</v>
       </c>
-      <c r="G11" s="6">
+      <c r="H11" s="6">
         <f>_xlfn.XLOOKUP(D11,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.37355851499999998</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="M11" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J11" s="6">
+      <c r="N11" s="6">
         <v>0.51720569999999999</v>
       </c>
-      <c r="K11" s="6">
+      <c r="O11" s="6">
         <v>0.51720569999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.79732053999999997</v>
       </c>
@@ -10810,24 +11888,27 @@
         <v>0.42048184333333333</v>
       </c>
       <c r="F12" s="6">
+        <v>0.17144337679947338</v>
+      </c>
+      <c r="G12" s="6">
         <f>_xlfn.XLOOKUP(D12,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.35937489250000004</v>
       </c>
-      <c r="G12" s="6">
+      <c r="H12" s="6">
         <f>_xlfn.XLOOKUP(D12,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.44670673666666671</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="M12" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="J12" s="6">
+      <c r="N12" s="6">
         <v>0.65199819999999997</v>
       </c>
-      <c r="K12" s="6">
+      <c r="O12" s="6">
         <v>0.27390003000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0.79732053999999997</v>
       </c>
@@ -10841,24 +11922,27 @@
         <v>0.46963706599999994</v>
       </c>
       <c r="F13" s="6">
+        <v>9.0011079301001176E-2</v>
+      </c>
+      <c r="G13" s="6">
         <f>_xlfn.XLOOKUP(D13,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.4636132</v>
       </c>
-      <c r="G13" s="6">
+      <c r="H13" s="6">
         <f>_xlfn.XLOOKUP(D13,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.40011453249999995</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="M13" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="J13" s="6">
+      <c r="N13" s="6">
         <v>0.93694025000000003</v>
       </c>
-      <c r="K13" s="6">
+      <c r="O13" s="6">
         <v>0.93694025000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0.79732053999999997</v>
       </c>
@@ -10872,24 +11956,27 @@
         <v>0.47241633999999999</v>
       </c>
       <c r="F14" s="6">
+        <v>0</v>
+      </c>
+      <c r="G14" s="6">
         <f>_xlfn.XLOOKUP(D14,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.31280202500000009</v>
       </c>
-      <c r="G14" s="6">
+      <c r="H14" s="6">
         <f>_xlfn.XLOOKUP(D14,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.63443416599999991</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="M14" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="J14" s="6">
+      <c r="N14" s="6">
         <v>0.54056070000000001</v>
       </c>
-      <c r="K14" s="6">
+      <c r="O14" s="6">
         <v>0.54041510000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.79732053999999997</v>
       </c>
@@ -10903,24 +11990,27 @@
         <v>0.49310513333333322</v>
       </c>
       <c r="F15" s="6">
+        <v>0.2826272345991353</v>
+      </c>
+      <c r="G15" s="6">
         <f>_xlfn.XLOOKUP(D15,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.50902492187500004</v>
       </c>
-      <c r="G15" s="6">
+      <c r="H15" s="6">
         <f>_xlfn.XLOOKUP(D15,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.50976659499999999</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="M15" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="J15" s="6">
+      <c r="N15" s="6">
         <v>0.85363259999999996</v>
       </c>
-      <c r="K15" s="6">
+      <c r="O15" s="6">
         <v>0.85363259999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.79732053999999997</v>
       </c>
@@ -10934,24 +12024,27 @@
         <v>0.51720569999999999</v>
       </c>
       <c r="F16" s="6">
+        <v>7.4505805969238281E-9</v>
+      </c>
+      <c r="G16" s="6">
         <f>_xlfn.XLOOKUP(D16,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.52480930000000003</v>
       </c>
-      <c r="G16" s="6">
+      <c r="H16" s="6">
         <f>_xlfn.XLOOKUP(D16,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.39641916999999999</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="M16" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="J16" s="6">
+      <c r="N16" s="6">
         <v>0.56027729999999998</v>
       </c>
-      <c r="K16" s="6">
+      <c r="O16" s="6">
         <v>0.32875618000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0.74763480000000004</v>
       </c>
@@ -10965,24 +12058,27 @@
         <v>0.52327754000000004</v>
       </c>
       <c r="F17" s="6">
+        <v>5.0532733208766417E-2</v>
+      </c>
+      <c r="G17" s="6">
         <f>_xlfn.XLOOKUP(D17,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.54014781090909103</v>
       </c>
-      <c r="G17" s="6">
+      <c r="H17" s="6">
         <f>_xlfn.XLOOKUP(D17,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.50971825733333342</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="M17" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="J17" s="6">
+      <c r="N17" s="6">
         <v>0.74094409999999999</v>
       </c>
-      <c r="K17" s="6">
+      <c r="O17" s="6">
         <v>0.19046825000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0.74763480000000004</v>
       </c>
@@ -10996,24 +12092,27 @@
         <v>0.52897513499999993</v>
       </c>
       <c r="F18" s="6">
+        <v>0.21190060519996243</v>
+      </c>
+      <c r="G18" s="6">
         <f>_xlfn.XLOOKUP(D18,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.52498712999999997</v>
       </c>
-      <c r="G18" s="6">
+      <c r="H18" s="6">
         <f>_xlfn.XLOOKUP(D18,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.59891786999999996</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="M18" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="J18" s="6">
+      <c r="N18" s="6">
         <v>0.57121710000000003</v>
       </c>
-      <c r="K18" s="6">
+      <c r="O18" s="6">
         <v>0.47533797999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0.74807674000000002</v>
       </c>
@@ -11027,24 +12126,27 @@
         <v>0.54044422000000003</v>
       </c>
       <c r="F19" s="6">
+        <v>6.5114300000450575E-5</v>
+      </c>
+      <c r="G19" s="6">
         <f>_xlfn.XLOOKUP(D19,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0</v>
       </c>
-      <c r="G19" s="6">
+      <c r="H19" s="6">
         <f>_xlfn.XLOOKUP(D19,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="M19" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="J19" s="6">
+      <c r="N19" s="6">
         <v>0.33157461999999999</v>
       </c>
-      <c r="K19" s="6">
+      <c r="O19" s="6">
         <v>0.31897335999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>0.74763480000000004</v>
       </c>
@@ -11058,24 +12160,27 @@
         <v>0.54412447500000005</v>
       </c>
       <c r="F20" s="6">
+        <v>4.2418924295067571E-2</v>
+      </c>
+      <c r="G20" s="6">
         <f>_xlfn.XLOOKUP(D20,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.54474180999999999</v>
       </c>
-      <c r="G20" s="6">
+      <c r="H20" s="6">
         <f>_xlfn.XLOOKUP(D20,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.51829862500000012</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="M20" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="J20" s="6">
+      <c r="N20" s="6">
         <v>0.91099799999999997</v>
       </c>
-      <c r="K20" s="6">
+      <c r="O20" s="6">
         <v>0.52656250000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>0.74763480000000004</v>
       </c>
@@ -11089,24 +12194,27 @@
         <v>0.56059696999999986</v>
       </c>
       <c r="F21" s="6">
+        <v>0.30269491228123901</v>
+      </c>
+      <c r="G21" s="6">
         <f>_xlfn.XLOOKUP(D21,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.57721637500000011</v>
       </c>
-      <c r="G21" s="6">
+      <c r="H21" s="6">
         <f>_xlfn.XLOOKUP(D21,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.62186232499999983</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="M21" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="J21" s="6">
+      <c r="N21" s="6">
         <v>0.79732053999999997</v>
       </c>
-      <c r="K21" s="6">
+      <c r="O21" s="6">
         <v>0.13503831999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>0.8991304</v>
       </c>
@@ -11120,24 +12228,27 @@
         <v>0.5862057850000002</v>
       </c>
       <c r="F22" s="6">
+        <v>0.2600582109894557</v>
+      </c>
+      <c r="G22" s="6">
         <f>_xlfn.XLOOKUP(D22,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.60809920904761883</v>
       </c>
-      <c r="G22" s="6">
+      <c r="H22" s="6">
         <f>_xlfn.XLOOKUP(D22,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.71322715500000045</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="M22" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="J22" s="6">
+      <c r="N22" s="6">
         <v>0.17677137000000001</v>
       </c>
-      <c r="K22" s="6">
+      <c r="O22" s="6">
         <v>0.17677137000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>0.8991304</v>
       </c>
@@ -11151,24 +12262,27 @@
         <v>0.68761579999999978</v>
       </c>
       <c r="F23" s="6">
+        <v>0.15647576116472142</v>
+      </c>
+      <c r="G23" s="6">
         <f>_xlfn.XLOOKUP(D23,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.68999980666666683</v>
       </c>
-      <c r="G23" s="6">
+      <c r="H23" s="6">
         <f>_xlfn.XLOOKUP(D23,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.66593574999999994</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="M23" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="J23" s="6">
+      <c r="N23" s="6">
         <v>0.73000169999999998</v>
       </c>
-      <c r="K23" s="6">
+      <c r="O23" s="6">
         <v>0.32794856999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>0.8991304</v>
       </c>
@@ -11182,24 +12296,27 @@
         <v>0.71568290000000001</v>
       </c>
       <c r="F24" s="6">
+        <v>0</v>
+      </c>
+      <c r="G24" s="6">
         <f>_xlfn.XLOOKUP(D24,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.70774870000000001</v>
       </c>
-      <c r="G24" s="6">
+      <c r="H24" s="6">
         <f>_xlfn.XLOOKUP(D24,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="M24" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="J24" s="6">
+      <c r="N24" s="6">
         <v>0.83646140000000002</v>
       </c>
-      <c r="K24" s="6">
+      <c r="O24" s="6">
         <v>0.15583521</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>0.8991304</v>
       </c>
@@ -11213,24 +12330,27 @@
         <v>0.7187802499999999</v>
       </c>
       <c r="F25" s="6">
+        <v>0.20261529890427685</v>
+      </c>
+      <c r="G25" s="6">
         <f>_xlfn.XLOOKUP(D25,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.90672759999999997</v>
       </c>
-      <c r="G25" s="6">
+      <c r="H25" s="6">
         <f>_xlfn.XLOOKUP(D25,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.63463328333333313</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="M25" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="J25" s="6">
+      <c r="N25" s="6">
         <v>0.85653679999999999</v>
       </c>
-      <c r="K25" s="6">
+      <c r="O25" s="6">
         <v>0.48967490000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>0.8991304</v>
       </c>
@@ -11244,24 +12364,27 @@
         <v>0.72708189999999984</v>
       </c>
       <c r="F26" s="6">
+        <v>9.6994750713005909E-2</v>
+      </c>
+      <c r="G26" s="6">
         <f>_xlfn.XLOOKUP(D26,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.72877930000000013</v>
       </c>
-      <c r="G26" s="6">
+      <c r="H26" s="6">
         <f>_xlfn.XLOOKUP(D26,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.73398845000000013</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="M26" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="J26" s="6">
+      <c r="N26" s="6">
         <v>0.47241633999999999</v>
       </c>
-      <c r="K26" s="6">
+      <c r="O26" s="6">
         <v>0.47241633999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>0.74094409999999999</v>
       </c>
@@ -11275,24 +12398,27 @@
         <v>0.73846215000000004</v>
       </c>
       <c r="F27" s="6">
+        <v>0</v>
+      </c>
+      <c r="G27" s="6">
         <f>_xlfn.XLOOKUP(D27,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.72207695000000005</v>
       </c>
-      <c r="G27" s="6">
+      <c r="H27" s="6">
         <f>_xlfn.XLOOKUP(D27,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.74895920000000005</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="M27" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="J27" s="6">
+      <c r="N27" s="6">
         <v>0.8991304</v>
       </c>
-      <c r="K27" s="6">
+      <c r="O27" s="6">
         <v>0.2322322</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>0.74094409999999999</v>
       </c>
@@ -11306,24 +12432,27 @@
         <v>0.76826452999999995</v>
       </c>
       <c r="F28" s="6">
+        <v>0</v>
+      </c>
+      <c r="G28" s="6">
         <f>_xlfn.XLOOKUP(D28,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.5468963</v>
       </c>
-      <c r="G28" s="6">
+      <c r="H28" s="6">
         <f>_xlfn.XLOOKUP(D28,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.75809943999999996</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="M28" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="J28" s="6">
+      <c r="N28" s="6">
         <v>0.86136365000000004</v>
       </c>
-      <c r="K28" s="6">
+      <c r="O28" s="6">
         <v>0.86136365000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>0.74094409999999999</v>
       </c>
@@ -11337,24 +12466,27 @@
         <v>0.85234225900000005</v>
       </c>
       <c r="F29" s="6">
+        <v>0.11027826239805079</v>
+      </c>
+      <c r="G29" s="6">
         <f>_xlfn.XLOOKUP(D29,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.85973333000000007</v>
       </c>
-      <c r="G29" s="6">
+      <c r="H29" s="6">
         <f>_xlfn.XLOOKUP(D29,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.8639597349999999</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="M29" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="J29" s="6">
+      <c r="N29" s="6">
         <v>0.43799232999999999</v>
       </c>
-      <c r="K29" s="6">
+      <c r="O29" s="6">
         <v>0.14425758999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>0.74094409999999999</v>
       </c>
@@ -11368,24 +12500,27 @@
         <v>0.85363259999999985</v>
       </c>
       <c r="F30" s="6">
+        <v>1.0536712127723509E-8</v>
+      </c>
+      <c r="G30" s="6">
         <f>_xlfn.XLOOKUP(D30,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.84493459999999998</v>
       </c>
-      <c r="G30" s="6">
+      <c r="H30" s="6">
         <f>_xlfn.XLOOKUP(D30,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.89763280000000001</v>
       </c>
-      <c r="I30" s="3" t="s">
+      <c r="M30" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="J30" s="6">
+      <c r="N30" s="6">
         <v>0.58436659999999996</v>
       </c>
-      <c r="K30" s="6">
+      <c r="O30" s="6">
         <v>0.50388235000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>0.74094409999999999</v>
       </c>
@@ -11399,24 +12534,27 @@
         <v>0.86136365000000004</v>
       </c>
       <c r="F31" s="6">
+        <v>0</v>
+      </c>
+      <c r="G31" s="6">
         <f>_xlfn.XLOOKUP(D31,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.86275720000000011</v>
       </c>
-      <c r="G31" s="6">
+      <c r="H31" s="6">
         <f>_xlfn.XLOOKUP(D31,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.88611550000000006</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="M31" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="J31" s="6">
+      <c r="N31" s="6">
         <v>0.73846215000000004</v>
       </c>
-      <c r="K31" s="6">
+      <c r="O31" s="6">
         <v>0.73846215000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>0.91099799999999997</v>
       </c>
@@ -11430,24 +12568,27 @@
         <v>0.93694024999999992</v>
       </c>
       <c r="F32" s="6">
+        <v>0</v>
+      </c>
+      <c r="G32" s="6">
         <f>_xlfn.XLOOKUP(D32,'[1]avg doc score'!$E:$E,'[1]avg doc score'!$F:$F,0)</f>
         <v>0.93206495</v>
       </c>
-      <c r="G32" s="6">
+      <c r="H32" s="6">
         <f>_xlfn.XLOOKUP(D32,'[2]avg doc score'!$E:$E,'[2]avg doc score'!$F:$F,0)</f>
         <v>0.52339156499999984</v>
       </c>
-      <c r="I32" s="3" t="s">
+      <c r="M32" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="J32" s="6">
+      <c r="N32" s="6">
         <v>0.76826452999999995</v>
       </c>
-      <c r="K32" s="6">
+      <c r="O32" s="6">
         <v>0.76826452999999995</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>0.91099799999999997</v>
       </c>
@@ -11460,25 +12601,28 @@
       <c r="E33" s="4">
         <v>0.51264732240677979</v>
       </c>
-      <c r="F33" s="9">
-        <f>AVERAGE(F3:F32)</f>
-        <v>0.48999196193883482</v>
+      <c r="F33" s="4">
+        <v>0.24632067657415488</v>
       </c>
       <c r="G33" s="9">
         <f>AVERAGE(G3:G32)</f>
+        <v>0.48999196193883482</v>
+      </c>
+      <c r="H33" s="9">
+        <f>AVERAGE(H3:H32)</f>
         <v>0.48519687959444452</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="M33" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="J33" s="6">
+      <c r="N33" s="6">
         <v>0.95696133000000005</v>
       </c>
-      <c r="K33" s="6">
+      <c r="O33" s="6">
         <v>0.10833058</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>0.91099799999999997</v>
       </c>
@@ -11486,7 +12630,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>0.91099799999999997</v>
       </c>
@@ -11494,7 +12638,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>0.91099799999999997</v>
       </c>
@@ -11514,7 +12658,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0.95696133000000005</v>
       </c>
@@ -11534,7 +12678,7 @@
         <v>0.14053692000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>0.95696133000000005</v>
       </c>
@@ -11554,7 +12698,7 @@
         <v>0.73398845000000013</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>0.95696133000000005</v>
       </c>
@@ -11574,7 +12718,7 @@
         <v>0.40059755499999994</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>0.95696133000000005</v>
       </c>
@@ -11594,7 +12738,7 @@
         <v>0.2380918345000001</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>0.95696133000000005</v>
       </c>
@@ -11614,7 +12758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>0.83646140000000002</v>
       </c>
@@ -11634,7 +12778,7 @@
         <v>0.8639597349999999</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>0.83646140000000002</v>
       </c>
@@ -11654,7 +12798,7 @@
         <v>0.24088813749999999</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>0.83646140000000002</v>
       </c>
@@ -11674,7 +12818,7 @@
         <v>0.60251958000000017</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>0.83646140000000002</v>
       </c>
@@ -11694,7 +12838,7 @@
         <v>0.39641916999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>0.83646140000000002</v>
       </c>
@@ -11714,7 +12858,7 @@
         <v>0.44670673666666671</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>0.47022631999999998</v>
       </c>
@@ -11734,7 +12878,7 @@
         <v>0.52339156499999984</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>0.47022631999999998</v>
       </c>

</xml_diff>